<commit_message>
registering 1st sprint day in burndown
</commit_message>
<xml_diff>
--- a/docs/management/Burndown/Burndown.xlsx
+++ b/docs/management/Burndown/Burndown.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\repositories\api-6-semestre\docs\management\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981443E1-A5C9-4FB1-BBB8-DE8F828D27AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075D881D-40BA-440A-A7F5-9FDDC3A6A52B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sprint 0" sheetId="2" r:id="rId1"/>
+    <sheet name="Tempo" sheetId="3" r:id="rId1"/>
+    <sheet name="Sprint 0" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Atividades</t>
   </si>
@@ -160,6 +161,30 @@
   </si>
   <si>
     <t>Média de horas por dia</t>
+  </si>
+  <si>
+    <t>Preço por hora</t>
+  </si>
+  <si>
+    <t>Quantidade de integrantes</t>
+  </si>
+  <si>
+    <t>Tempo diário</t>
+  </si>
+  <si>
+    <t>Quantidade de dias</t>
+  </si>
+  <si>
+    <t>Total horas sprint</t>
+  </si>
+  <si>
+    <t>Total custo sprint</t>
+  </si>
+  <si>
+    <t>Total horas projeto</t>
+  </si>
+  <si>
+    <t>Total custo projeto</t>
   </si>
 </sst>
 </file>
@@ -273,7 +298,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,12 +327,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,6 +358,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,64 +479,64 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>141</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>141</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>141</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>141</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>133</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>133</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>43</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>43</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>34</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>34</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>364.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -545,67 +573,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>139.04761904761904</c:v>
+                  <c:v>350</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>132.09523809523807</c:v>
+                  <c:v>332.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>125.14285714285712</c:v>
+                  <c:v>315</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>118.19047619047618</c:v>
+                  <c:v>297.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>111.23809523809523</c:v>
+                  <c:v>280</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>104.28571428571428</c:v>
+                  <c:v>262.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>97.333333333333329</c:v>
+                  <c:v>245</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>90.38095238095238</c:v>
+                  <c:v>227.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>83.428571428571431</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>76.476190476190482</c:v>
+                  <c:v>192.5</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>69.523809523809533</c:v>
+                  <c:v>175</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>62.571428571428584</c:v>
+                  <c:v>157.5</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>55.619047619047635</c:v>
+                  <c:v>140</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>48.666666666666686</c:v>
+                  <c:v>122.5</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>41.714285714285737</c:v>
+                  <c:v>105</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.761904761904788</c:v>
+                  <c:v>87.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.809523809523835</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.857142857142883</c:v>
+                  <c:v>52.5</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>13.90476190476193</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.9523809523809774</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.4868995751603507E-14</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1709,13 +1737,118 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECB3CFB-FAFD-448D-BA08-3C7BDBA6E633}">
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" s="24"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="24">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="24">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="24">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="24">
+        <f>B3*B4*B5</f>
+        <v>367.5</v>
+      </c>
+      <c r="C6">
+        <f>B6/7</f>
+        <v>52.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="24">
+        <f>B2*B6</f>
+        <v>18375</v>
+      </c>
+      <c r="C7">
+        <f>B7/7</f>
+        <v>2625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B8" s="24">
+        <f>B6*4</f>
+        <v>1470</v>
+      </c>
+      <c r="C8">
+        <f>B8/7</f>
+        <v>210</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" s="24">
+        <f>B7*4</f>
+        <v>73500</v>
+      </c>
+      <c r="C9">
+        <f>B9/7</f>
+        <v>10500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B4BA60-9604-4D54-BDB3-BA720851CBCD}">
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:W24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E16" sqref="E16"/>
+      <selection pane="topRight" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1728,39 +1861,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
+      <c r="A2" s="23"/>
+      <c r="B2" s="23"/>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1826,8 +1959,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="12"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -1958,15 +2091,13 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="3">
-        <v>8</v>
-      </c>
+      <c r="G6" s="3"/>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
       <c r="J6" s="3"/>
@@ -1990,10 +2121,11 @@
       </c>
       <c r="B7" s="3">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>5</v>
+        <f>0.5+0.5</f>
+        <v>1</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="3"/>
@@ -2022,7 +2154,7 @@
       </c>
       <c r="B8" s="3">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -2032,9 +2164,7 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
-      <c r="K8" s="3">
-        <v>9</v>
-      </c>
+      <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -2054,9 +2184,11 @@
       </c>
       <c r="B9" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
+        <v>0.25</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.25</v>
+      </c>
       <c r="D9" s="3"/>
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
@@ -2084,7 +2216,7 @@
       </c>
       <c r="B10" s="3">
         <f t="shared" si="0"/>
-        <v>105</v>
+        <v>0</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -2092,17 +2224,13 @@
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3"/>
-      <c r="I10" s="3">
-        <v>90</v>
-      </c>
+      <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
       <c r="L10" s="3"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
-      <c r="O10" s="3">
-        <v>15</v>
-      </c>
+      <c r="O10" s="3"/>
       <c r="P10" s="3"/>
       <c r="Q10" s="3"/>
       <c r="R10" s="3"/>
@@ -2178,9 +2306,11 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="C13" s="3"/>
+        <v>1.5</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1.5</v>
+      </c>
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
@@ -2208,87 +2338,87 @@
       </c>
       <c r="B14" s="5">
         <f>B15</f>
-        <v>146</v>
+        <v>367.5</v>
       </c>
       <c r="C14" s="3">
         <f>B15-SUM(C4:C13)</f>
-        <v>141</v>
+        <v>364.75</v>
       </c>
       <c r="D14" s="3">
         <f>C14-SUM(D4:D13)</f>
-        <v>141</v>
+        <v>364.75</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ref="E14:V14" si="1">D14-SUM(E4:E13)</f>
-        <v>141</v>
+        <v>364.75</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>141</v>
+        <v>364.75</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>364.75</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>133</v>
+        <v>364.75</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>364.75</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>364.75</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>364.75</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>364.75</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>364.75</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>34</v>
+        <v>364.75</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="R14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="T14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="1"/>
-        <v>19</v>
+        <v>364.75</v>
       </c>
       <c r="W14" s="3"/>
     </row>
@@ -2297,167 +2427,167 @@
         <v>34</v>
       </c>
       <c r="B15" s="10">
-        <f>SUM(D18:D20)</f>
-        <v>146</v>
+        <f>Tempo!B6</f>
+        <v>367.5</v>
       </c>
       <c r="C15" s="3">
         <f>B15-B24</f>
-        <v>139.04761904761904</v>
+        <v>350</v>
       </c>
       <c r="D15" s="3">
         <f>C15-B24</f>
-        <v>132.09523809523807</v>
+        <v>332.5</v>
       </c>
       <c r="E15" s="3">
         <f>D15-B24</f>
-        <v>125.14285714285712</v>
+        <v>315</v>
       </c>
       <c r="F15" s="3">
         <f>E15-B24</f>
-        <v>118.19047619047618</v>
+        <v>297.5</v>
       </c>
       <c r="G15" s="3">
         <f>F15-B24</f>
-        <v>111.23809523809523</v>
+        <v>280</v>
       </c>
       <c r="H15" s="3">
         <f>G15-B24</f>
-        <v>104.28571428571428</v>
+        <v>262.5</v>
       </c>
       <c r="I15" s="3">
         <f>H15-B24</f>
-        <v>97.333333333333329</v>
+        <v>245</v>
       </c>
       <c r="J15" s="3">
         <f>I15-B24</f>
-        <v>90.38095238095238</v>
+        <v>227.5</v>
       </c>
       <c r="K15" s="3">
         <f>J15-B24</f>
-        <v>83.428571428571431</v>
+        <v>210</v>
       </c>
       <c r="L15" s="3">
         <f>K15-B24</f>
-        <v>76.476190476190482</v>
+        <v>192.5</v>
       </c>
       <c r="M15" s="3">
         <f>L15-B24</f>
-        <v>69.523809523809533</v>
+        <v>175</v>
       </c>
       <c r="N15" s="3">
         <f>M15-B24</f>
-        <v>62.571428571428584</v>
+        <v>157.5</v>
       </c>
       <c r="O15" s="3">
         <f>N15-B24</f>
-        <v>55.619047619047635</v>
+        <v>140</v>
       </c>
       <c r="P15" s="3">
         <f>O15-B24</f>
-        <v>48.666666666666686</v>
+        <v>122.5</v>
       </c>
       <c r="Q15" s="3">
         <f>P15-B24</f>
-        <v>41.714285714285737</v>
+        <v>105</v>
       </c>
       <c r="R15" s="3">
         <f>Q15-B24</f>
-        <v>34.761904761904788</v>
+        <v>87.5</v>
       </c>
       <c r="S15" s="3">
         <f>R15-B24</f>
-        <v>27.809523809523835</v>
+        <v>70</v>
       </c>
       <c r="T15" s="3">
         <f>S15-B24</f>
-        <v>20.857142857142883</v>
+        <v>52.5</v>
       </c>
       <c r="U15" s="3">
         <f>T15-B24</f>
-        <v>13.90476190476193</v>
+        <v>35</v>
       </c>
       <c r="V15" s="3">
         <f>U15-B24</f>
-        <v>6.9523809523809774</v>
+        <v>17.5</v>
       </c>
       <c r="W15" s="3">
         <f>IF(V15-B24&lt;0,0,V15-B24)</f>
-        <v>2.4868995751603507E-14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="17" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B18" s="14">
+      <c r="B18" s="12">
         <v>5</v>
       </c>
-      <c r="C18" s="14">
-        <v>16</v>
+      <c r="C18" s="12">
+        <v>4</v>
       </c>
       <c r="D18" s="3">
         <f>B18*C18</f>
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="14">
+      <c r="B19" s="12">
         <v>5</v>
       </c>
-      <c r="C19" s="14">
-        <v>6</v>
+      <c r="C19" s="12">
+        <v>2</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" ref="D19:D20" si="2">B19*C19</f>
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="20" t="s">
+      <c r="A20" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B20" s="14">
+      <c r="B20" s="12">
         <v>9</v>
       </c>
-      <c r="C20" s="14">
-        <v>4</v>
+      <c r="C20" s="12">
+        <v>1</v>
       </c>
       <c r="D20" s="3">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" s="22"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="13"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="19"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="11"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B22" s="14">
+      <c r="B22" s="12">
         <f>COUNTA(C3:W3)</f>
         <v>21</v>
       </c>
-      <c r="C22" s="21"/>
-      <c r="D22" s="13"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="11"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
@@ -2465,7 +2595,7 @@
       </c>
       <c r="B24" s="9">
         <f>B15/B22</f>
-        <v>6.9523809523809526</v>
+        <v>17.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding new finished tasks
</commit_message>
<xml_diff>
--- a/docs/management/Burndown/Burndown.xlsx
+++ b/docs/management/Burndown/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\repositories\api-6-semestre\docs\management\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB365D3-6A1E-47B4-BC53-31010A4B5995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39E271F4-0859-493D-8A7B-4066929366DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,52 +488,52 @@
                   <c:v>258.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>242.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>258.29000000000002</c:v>
+                  <c:v>235.29000000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1845,7 +1845,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="B6" s="3">
         <f t="shared" si="0"/>
-        <v>7.63</v>
+        <v>14.629999999999999</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -2102,7 +2102,9 @@
         <v>4</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
+      <c r="I6" s="3">
+        <v>7</v>
+      </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
@@ -2314,7 +2316,7 @@
       </c>
       <c r="B13" s="3">
         <f t="shared" si="0"/>
-        <v>20.5</v>
+        <v>36.5</v>
       </c>
       <c r="C13" s="3">
         <f>1.5+14 +N("Obs.: 14 horas por conta do que foi gastado de horas no final de semana")</f>
@@ -2329,7 +2331,9 @@
       <c r="G13" s="3">
         <v>4</v>
       </c>
-      <c r="H13" s="3"/>
+      <c r="H13" s="3">
+        <v>16</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -2376,67 +2380,67 @@
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>242.29000000000002</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="R14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="T14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
       <c r="W14" s="3">
         <f t="shared" si="1"/>
-        <v>258.29000000000002</v>
+        <v>235.29000000000002</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
improving burndown style and updating time effort
</commit_message>
<xml_diff>
--- a/docs/management/Burndown/Burndown.xlsx
+++ b/docs/management/Burndown/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\port3\repositories\api-6-semestre\docs\management\Burndown\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C659ACA-AF84-465A-A797-651116D30865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FBAABE2-5239-44D6-830E-5FE200535FAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -313,13 +313,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -426,6 +426,144 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 0'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>29/08</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>31/08</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>03/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>04/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>05/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>06/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>07/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>08/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>09/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10/09</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>11/09</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>12/09</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>13/09</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>14/09</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>15/09</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>16/09</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>17/09</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>18/09</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Sprint 0'!$C$14:$W$14</c:f>
@@ -433,67 +571,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>83.25</c:v>
+                  <c:v>133.25</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.25</c:v>
+                  <c:v>128.25</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.62</c:v>
+                  <c:v>124.62</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>72.290000000000006</c:v>
+                  <c:v>122.29</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>64.290000000000006</c:v>
+                  <c:v>114.29</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>48.290000000000006</c:v>
+                  <c:v>98.29</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>41.290000000000006</c:v>
+                  <c:v>91.29</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>40.790000000000006</c:v>
+                  <c:v>90.79</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>29.790000000000006</c:v>
+                  <c:v>79.790000000000006</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -523,6 +661,144 @@
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>'Sprint 0'!$C$2:$W$3</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="21"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>4</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>8</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>10</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>11</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>12</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>13</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>14</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>15</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>16</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>17</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>18</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>19</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>20</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>21</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>29/08</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>30/08</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>31/08</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>01/09</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>02/09</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>03/09</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>04/09</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>05/09</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>06/09</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>07/09</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>08/09</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>09/09</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>10/09</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>11/09</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>12/09</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>13/09</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>14/09</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>15/09</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>16/09</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>17/09</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>18/09</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>'Sprint 0'!$C$15:$W$15</c:f>
@@ -530,67 +806,67 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>95.238095238095241</c:v>
+                  <c:v>142.85714285714286</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>90.476190476190482</c:v>
+                  <c:v>135.71428571428572</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.714285714285722</c:v>
+                  <c:v>128.57142857142858</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80.952380952380963</c:v>
+                  <c:v>121.42857142857144</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76.190476190476204</c:v>
+                  <c:v>114.28571428571431</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>71.428571428571445</c:v>
+                  <c:v>107.14285714285717</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>66.666666666666686</c:v>
+                  <c:v>100.00000000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>61.904761904761926</c:v>
+                  <c:v>92.85714285714289</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>57.142857142857167</c:v>
+                  <c:v>85.714285714285751</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.380952380952408</c:v>
+                  <c:v>78.571428571428612</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47.619047619047649</c:v>
+                  <c:v>71.428571428571473</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42.85714285714289</c:v>
+                  <c:v>64.285714285714334</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>38.09523809523813</c:v>
+                  <c:v>57.142857142857189</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>33.333333333333371</c:v>
+                  <c:v>50.000000000000043</c:v>
                 </c:pt>
                 <c:pt idx="14">
+                  <c:v>42.857142857142897</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>35.714285714285751</c:v>
+                </c:pt>
+                <c:pt idx="16">
                   <c:v>28.571428571428608</c:v>
                 </c:pt>
-                <c:pt idx="15">
-                  <c:v>23.809523809523846</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>19.047619047619083</c:v>
-                </c:pt>
                 <c:pt idx="17">
-                  <c:v>14.28571428571432</c:v>
+                  <c:v>21.428571428571466</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.5238095238095575</c:v>
+                  <c:v>14.285714285714324</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4.7619047619047956</c:v>
+                  <c:v>7.1428571428571805</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.3750779948604759E-14</c:v>
+                  <c:v>3.730349362740526E-14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -621,6 +897,34 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -674,6 +978,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -753,8 +1058,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US" b="1"/>
-                  <a:t>Quantidade de tarefas</a:t>
+                  <a:t>Quantidade de</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" b="1" baseline="0"/>
+                  <a:t> esforço</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" b="1"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1461,15 +1771,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>246138</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>36588</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>78318</xdr:colOff>
-      <xdr:row>41</xdr:row>
-      <xdr:rowOff>2872</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1698,7 +2008,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1734,16 +2044,15 @@
       <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="17">
-        <f>100</f>
-        <v>100</v>
+      <c r="B4" s="15">
+        <v>150</v>
       </c>
       <c r="C4" s="12">
         <f>B4/7</f>
-        <v>14.285714285714286</v>
+        <v>21.428571428571427</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1752,11 +2061,11 @@
       </c>
       <c r="B5" s="12">
         <f>B2*B4</f>
-        <v>5000</v>
+        <v>7500</v>
       </c>
       <c r="C5" s="12">
         <f>B5/7</f>
-        <v>714.28571428571433</v>
+        <v>1071.4285714285713</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1765,11 +2074,11 @@
       </c>
       <c r="B6" s="12">
         <f>B4*4</f>
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="C6" s="12">
         <f>B6/7</f>
-        <v>57.142857142857146</v>
+        <v>85.714285714285708</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1778,11 +2087,11 @@
       </c>
       <c r="B7" s="12">
         <f>B5*4</f>
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="C7" s="12">
         <f>B7/7</f>
-        <v>2857.1428571428573</v>
+        <v>4285.7142857142853</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1790,10 +2099,13 @@
         <v>40</v>
       </c>
       <c r="B8" s="12">
-        <f>B4/B3</f>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="C8" s="12"/>
+        <f>B4/B9</f>
+        <v>7.1428571428571432</v>
+      </c>
+      <c r="C8" s="12">
+        <f>B8/7</f>
+        <v>1.0204081632653061</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="12" t="s">
@@ -1814,9 +2126,9 @@
   <sheetPr codeName="Planilha1"/>
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="E1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1829,39 +2141,39 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A2" s="16"/>
-      <c r="B2" s="16"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
       <c r="C2" s="1" t="s">
         <v>12</v>
       </c>
@@ -1927,8 +2239,8 @@
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A3" s="16"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
       <c r="C3" s="2">
         <v>1</v>
       </c>
@@ -2331,91 +2643,91 @@
       </c>
       <c r="B14" s="5">
         <f>B15</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C14" s="3">
         <f>B15-SUM(C4:C13)</f>
-        <v>83.25</v>
+        <v>133.25</v>
       </c>
       <c r="D14" s="3">
         <f>C14-SUM(D4:D13)</f>
-        <v>78.25</v>
+        <v>128.25</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ref="E14:W14" si="1">D14-SUM(E4:E13)</f>
-        <v>74.62</v>
+        <v>124.62</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" si="1"/>
-        <v>72.290000000000006</v>
+        <v>122.29</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" si="1"/>
-        <v>64.290000000000006</v>
+        <v>114.29</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" si="1"/>
-        <v>48.290000000000006</v>
+        <v>98.29</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" si="1"/>
-        <v>41.290000000000006</v>
+        <v>91.29</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" si="1"/>
-        <v>40.790000000000006</v>
+        <v>90.79</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="L14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="N14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="O14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="P14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="Q14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="R14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="S14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="T14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="U14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="V14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
       <c r="W14" s="3">
         <f t="shared" si="1"/>
-        <v>29.790000000000006</v>
+        <v>79.790000000000006</v>
       </c>
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.2">
@@ -2424,91 +2736,91 @@
       </c>
       <c r="B15" s="10">
         <f>Tempo!B4</f>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="C15" s="3">
         <f>B15-B20</f>
-        <v>95.238095238095241</v>
+        <v>142.85714285714286</v>
       </c>
       <c r="D15" s="3">
         <f>C15-B20</f>
-        <v>90.476190476190482</v>
+        <v>135.71428571428572</v>
       </c>
       <c r="E15" s="3">
         <f>D15-B20</f>
-        <v>85.714285714285722</v>
+        <v>128.57142857142858</v>
       </c>
       <c r="F15" s="3">
         <f>E15-B20</f>
-        <v>80.952380952380963</v>
+        <v>121.42857142857144</v>
       </c>
       <c r="G15" s="3">
         <f>F15-B20</f>
-        <v>76.190476190476204</v>
+        <v>114.28571428571431</v>
       </c>
       <c r="H15" s="3">
         <f>G15-B20</f>
-        <v>71.428571428571445</v>
+        <v>107.14285714285717</v>
       </c>
       <c r="I15" s="3">
         <f>H15-B20</f>
-        <v>66.666666666666686</v>
+        <v>100.00000000000003</v>
       </c>
       <c r="J15" s="3">
         <f>I15-B20</f>
-        <v>61.904761904761926</v>
+        <v>92.85714285714289</v>
       </c>
       <c r="K15" s="3">
         <f>J15-B20</f>
-        <v>57.142857142857167</v>
+        <v>85.714285714285751</v>
       </c>
       <c r="L15" s="3">
         <f>K15-B20</f>
-        <v>52.380952380952408</v>
+        <v>78.571428571428612</v>
       </c>
       <c r="M15" s="3">
         <f>L15-B20</f>
-        <v>47.619047619047649</v>
+        <v>71.428571428571473</v>
       </c>
       <c r="N15" s="3">
         <f>M15-B20</f>
-        <v>42.85714285714289</v>
+        <v>64.285714285714334</v>
       </c>
       <c r="O15" s="3">
         <f>N15-B20</f>
-        <v>38.09523809523813</v>
+        <v>57.142857142857189</v>
       </c>
       <c r="P15" s="3">
         <f>O15-B20</f>
-        <v>33.333333333333371</v>
+        <v>50.000000000000043</v>
       </c>
       <c r="Q15" s="3">
         <f>P15-B20</f>
-        <v>28.571428571428608</v>
+        <v>42.857142857142897</v>
       </c>
       <c r="R15" s="3">
         <f>Q15-B20</f>
-        <v>23.809523809523846</v>
+        <v>35.714285714285751</v>
       </c>
       <c r="S15" s="3">
         <f>R15-B20</f>
-        <v>19.047619047619083</v>
+        <v>28.571428571428608</v>
       </c>
       <c r="T15" s="3">
         <f>S15-B20</f>
-        <v>14.28571428571432</v>
+        <v>21.428571428571466</v>
       </c>
       <c r="U15" s="3">
         <f>T15-B20</f>
-        <v>9.5238095238095575</v>
+        <v>14.285714285714324</v>
       </c>
       <c r="V15" s="3">
         <f>U15-B20</f>
-        <v>4.7619047619047956</v>
+        <v>7.1428571428571805</v>
       </c>
       <c r="W15" s="3">
         <f>IF(V15-B20&lt;0,0,V15-B20)</f>
-        <v>3.3750779948604759E-14</v>
+        <v>3.730349362740526E-14</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2534,7 +2846,7 @@
       </c>
       <c r="B20" s="9">
         <f>B15/B18</f>
-        <v>4.7619047619047619</v>
+        <v>7.1428571428571432</v>
       </c>
     </row>
   </sheetData>

</xml_diff>